<commit_message>
added structure render and modified expenses
</commit_message>
<xml_diff>
--- a/expenses.xlsx
+++ b/expenses.xlsx
@@ -2,19 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\augu\Stephano\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\__STEFANO__\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7656"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,9 +23,44 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+  <si>
+    <t>COMPONENTS</t>
+  </si>
+  <si>
+    <t>ADARSH</t>
+  </si>
+  <si>
+    <t>AUGUSTINE</t>
+  </si>
+  <si>
+    <t>KURIAN</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Motor 1</t>
+  </si>
+  <si>
+    <t>Motor 2</t>
+  </si>
+  <si>
+    <t>Motor 3</t>
+  </si>
+  <si>
+    <t>Motor 4</t>
+  </si>
+  <si>
+    <t>Sensor MPU6050</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -33,16 +68,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -50,14 +106,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Calculation" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -336,14 +421,151 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1">
+        <v>900</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <f>(B2+C2+D2)</f>
+        <v>900</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>900</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <f>(B3+C3+D3)</f>
+        <v>900</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>900</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" ref="E4:E7" si="0">(B4+C4+D4)</f>
+        <v>900</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>900</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1">
+        <v>300</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="2">
+        <f>SUM(B2:B6)</f>
+        <v>1200</v>
+      </c>
+      <c r="C10" s="2">
+        <f>SUM(C2:C6)</f>
+        <v>1800</v>
+      </c>
+      <c r="D10" s="2">
+        <f>SUM(D2:D6)</f>
+        <v>900</v>
+      </c>
+      <c r="E10" s="4">
+        <f>SUM(E2:E6)</f>
+        <v>3900</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>